<commit_message>
Added new ui script files
</commit_message>
<xml_diff>
--- a/PythonWorkingScripts_InputData/Assessment/plagiarism_report/plagiarism_report.xlsx
+++ b/PythonWorkingScripts_InputData/Assessment/plagiarism_report/plagiarism_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t>Candidate Id</t>
   </si>
@@ -52,20 +52,74 @@
     <t>Diff Url</t>
   </si>
   <si>
-    <t>Candidate 006</t>
-  </si>
-  <si>
-    <t>Not found</t>
-  </si>
-  <si>
-    <t>Candidate 001</t>
+    <t>Muthu Plag One</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_7b05e954-e56a-43b3-a278-47f85a167be3.html</t>
+  </si>
+  <si>
+    <t>Muthu Plag Three</t>
+  </si>
+  <si>
+    <t>Muthu Plag Two</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_b1b0b4be-ba5a-4ec6-9748-1ad0513322d2.html</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_fa234021-da6b-41b9-b36a-4c66cbddf925.html</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_127b13b9-c0d3-4744-b875-74d01561327a.html</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_f1a68e40-ea08-4b01-ba8f-3f83b0b46ac2.html</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_828e40dd-0ad9-4c0a-ae82-3d23187b87fb.html</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_731dde2e-3167-49df-a9be-fc76a889161f.html</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_8afe5494-5995-4da5-a7c6-69d2cc5dd141.html</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_3f11b8b4-3144-4b57-b1dd-ae50e2452f92.html</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_32e8e8d8-7882-475d-a67d-a31fe5e9bc88.html</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_3abbeadd-de4a-4fe5-90d4-e9657ff968e5.html</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_80967e2b-895a-4931-98cb-c8e5309569e2.html</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_34ef5bbe-b05b-406e-8e66-dfb4d7a16871.html</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_651654f9-b9ac-40b7-9ecd-6a063a6f7327.html</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_d1a8b36c-53b1-441d-8b28-2aabce1d4d7e.html</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_afff1efa-9aca-4625-bd81-642f82a74513.html</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_08d22aed-7f81-4ac5-a603-4ab0175c169c.html</t>
+  </si>
+  <si>
+    <t>https://s3-ap-southeast-1.amazonaws.com/ams-in-self-expiring-files/30-720h/Automation/candidatetranscript/diff_16b30cdb-e025-46f9-8efb-5db5a0dc9f13.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +131,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,11 +164,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,45 +513,655 @@
     </row>
     <row r="2" spans="1:12" ht="20" customHeight="1">
       <c r="A2">
-        <v>1308606</v>
+        <v>1309057</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2">
-        <v>118397</v>
+        <v>120761</v>
       </c>
       <c r="D2">
-        <v>0.8</v>
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
       </c>
       <c r="F2">
-        <v>6</v>
-      </c>
-      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1309061</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="20" customHeight="1">
       <c r="A3">
-        <v>1308608</v>
+        <v>1309059</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <v>118397</v>
+        <v>120761</v>
       </c>
       <c r="D3">
-        <v>1.2</v>
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
       </c>
       <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>1309061</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="20" customHeight="1">
+      <c r="A4">
+        <v>1309061</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>120761</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>1309059</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="20" customHeight="1">
+      <c r="A5">
+        <v>1309057</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>120763</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
         <v>1</v>
       </c>
-      <c r="K3" t="s">
-        <v>13</v>
+      <c r="G5">
+        <v>1309061</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="20" customHeight="1">
+      <c r="A6">
+        <v>1309059</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>120763</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1309061</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="20" customHeight="1">
+      <c r="A7">
+        <v>1309061</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>120763</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>1309059</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="20" customHeight="1">
+      <c r="A8">
+        <v>1309057</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>120765</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>65.11628</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1309061</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8">
+        <v>20</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="20" customHeight="1">
+      <c r="A9">
+        <v>1309059</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>120765</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>64.40678</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>1309061</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9">
+        <v>20</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="20" customHeight="1">
+      <c r="A10">
+        <v>1309061</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>120765</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>65.11628</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>1309057</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10">
+        <v>20</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="20" customHeight="1">
+      <c r="A11">
+        <v>1309057</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>120767</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>66.666664</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1309061</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11">
+        <v>20</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="20" customHeight="1">
+      <c r="A12">
+        <v>1309059</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>120767</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>48.648647</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>1309061</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12">
+        <v>20</v>
+      </c>
+      <c r="J12">
+        <v>3</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="20" customHeight="1">
+      <c r="A13">
+        <v>1309061</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>120767</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>66.666664</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>1309057</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13">
+        <v>20</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="20" customHeight="1">
+      <c r="A14">
+        <v>1309057</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>120769</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>71.42857</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1309061</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14">
+        <v>20</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="20" customHeight="1">
+      <c r="A15">
+        <v>1309059</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>120769</v>
+      </c>
+      <c r="D15">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>80.597015</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>1309061</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15">
+        <v>20</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="20" customHeight="1">
+      <c r="A16">
+        <v>1309061</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>120769</v>
+      </c>
+      <c r="D16">
+        <v>20</v>
+      </c>
+      <c r="E16">
+        <v>80.597015</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>1309059</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16">
+        <v>20</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="20" customHeight="1">
+      <c r="A17">
+        <v>1309057</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>120771</v>
+      </c>
+      <c r="D17">
+        <v>20</v>
+      </c>
+      <c r="E17">
+        <v>55.172413</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1309061</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17">
+        <v>20</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="20" customHeight="1">
+      <c r="A18">
+        <v>1309059</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>120771</v>
+      </c>
+      <c r="D18">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>84</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>1309061</v>
+      </c>
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18">
+        <v>20</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="20" customHeight="1">
+      <c r="A19">
+        <v>1309061</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>120771</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
+      <c r="E19">
+        <v>84</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>1309059</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19">
+        <v>20</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L3" r:id="rId2"/>
+    <hyperlink ref="L4" r:id="rId3"/>
+    <hyperlink ref="L5" r:id="rId4"/>
+    <hyperlink ref="L6" r:id="rId5"/>
+    <hyperlink ref="L7" r:id="rId6"/>
+    <hyperlink ref="L8" r:id="rId7"/>
+    <hyperlink ref="L9" r:id="rId8"/>
+    <hyperlink ref="L10" r:id="rId9"/>
+    <hyperlink ref="L11" r:id="rId10"/>
+    <hyperlink ref="L12" r:id="rId11"/>
+    <hyperlink ref="L13" r:id="rId12"/>
+    <hyperlink ref="L14" r:id="rId13"/>
+    <hyperlink ref="L15" r:id="rId14"/>
+    <hyperlink ref="L16" r:id="rId15"/>
+    <hyperlink ref="L17" r:id="rId16"/>
+    <hyperlink ref="L18" r:id="rId17"/>
+    <hyperlink ref="L19" r:id="rId18"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>